<commit_message>
Ajout de type pour le model logique 07ba857a864e5ebd288ece40bdf75db2511d8871
</commit_message>
<xml_diff>
--- a/add-info-dmp/ig/StructureDefinition-AuthorInstitution.xlsx
+++ b/add-info-dmp/ig/StructureDefinition-AuthorInstitution.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-05-02T13:48:57+00:00</t>
+    <t>2025-05-02T14:15:44+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -275,7 +275,7 @@
     <t>AuthorInstitution.10</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension {elementdefinition-identifier}
+    <t xml:space="preserve">integer {https://interop.esante.gouv.fr/ig/fhir/pdsm4dmp/StructureDefinition/StructIdNat}
 </t>
   </si>
   <si>
@@ -603,7 +603,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="32.609375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="71.6875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>